<commit_message>
Merging st Paul class 1
</commit_message>
<xml_diff>
--- a/Tools/Find participant tool.xlsx
+++ b/Tools/Find participant tool.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5D271F-1929-4EF3-895B-3583EB56F6F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F05FEB7-BE68-433C-ABF2-69BEF939F968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5884" uniqueCount="1381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5904" uniqueCount="1388">
   <si>
     <t>راضي</t>
   </si>
@@ -4219,13 +4219,34 @@
   </si>
   <si>
     <t>01270444433</t>
+  </si>
+  <si>
+    <t>01207620600</t>
+  </si>
+  <si>
+    <t>01273421732</t>
+  </si>
+  <si>
+    <t>01282912158</t>
+  </si>
+  <si>
+    <t>01279097016</t>
+  </si>
+  <si>
+    <t>01224143525</t>
+  </si>
+  <si>
+    <t>01210144305</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4270,6 +4291,13 @@
       <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -4341,7 +4369,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4373,6 +4401,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -4380,23 +4409,7 @@
     <cellStyle name="Normal_Classes" xfId="2" xr:uid="{11E951F3-3E42-4D45-99D7-E0B87551DEE2}"/>
     <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{B6ECA741-77A3-4418-94B5-152DA9FB3C57}"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF00FF"/>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF00FF"/>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill>
@@ -4405,25 +4418,7 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -5389,9 +5384,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -5408,12 +5400,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E9DDE7AD-5515-4F83-8F50-C3AB41885269}" name="Table2" displayName="Table2" ref="A1:F36" totalsRowShown="0" headerRowDxfId="36">
-  <autoFilter ref="A1:F36" xr:uid="{E9DDE7AD-5515-4F83-8F50-C3AB41885269}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E9DDE7AD-5515-4F83-8F50-C3AB41885269}" name="Table2" displayName="Table2" ref="A1:F46" totalsRowShown="0" headerRowDxfId="31">
+  <autoFilter ref="A1:F46" xr:uid="{E9DDE7AD-5515-4F83-8F50-C3AB41885269}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1B0FC3C9-6395-4A54-8F48-F8E83AB846DC}" name="الاسم"/>
     <tableColumn id="2" xr3:uid="{040B6D61-E04D-4AE0-BE39-22A9A6F6BDDB}" name="رقم التليفون"/>
-    <tableColumn id="3" xr3:uid="{275C1BA1-3853-4BCC-9432-3CB61CB0E6B2}" name="اللي لقيته" dataDxfId="35">
+    <tableColumn id="3" xr3:uid="{275C1BA1-3853-4BCC-9432-3CB61CB0E6B2}" name="اللي لقيته" dataDxfId="1">
       <calculatedColumnFormula array="1">IF(_xlfn.XLOOKUP(B2,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B2,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B2,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B2,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B2,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B2,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B2,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B2,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B2,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A2&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{3C3972B0-F6D7-492F-909C-5B0542BD13AD}" name="ID">
@@ -5422,7 +5414,7 @@
     <tableColumn id="5" xr3:uid="{48FB2210-5F4C-426A-BDC1-B3355AD6F297}" name="الاسم اللي لقيته">
       <calculatedColumnFormula>IF(D2&lt;&gt;"",LOOKUP(D2,Table1[ID],Table1[fname]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C1BB6043-A545-4881-A271-028026FAD3B1}" name="الفصل" dataDxfId="34">
+    <tableColumn id="6" xr3:uid="{C1BB6043-A545-4881-A271-028026FAD3B1}" name="الفصل" dataDxfId="30">
       <calculatedColumnFormula>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5431,30 +5423,30 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A8F3280-CF74-42C5-B84F-1B481A234B39}" name="Table1" displayName="Table1" ref="A1:U305" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29" headerRowCellStyle="Normal_Sheet1" dataCellStyle="Normal_Sheet1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A8F3280-CF74-42C5-B84F-1B481A234B39}" name="Table1" displayName="Table1" ref="A1:U305" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25" headerRowCellStyle="Normal_Sheet1" dataCellStyle="Normal_Sheet1">
   <autoFilter ref="A1:U305" xr:uid="{3A8F3280-CF74-42C5-B84F-1B481A234B39}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{56277AF5-8907-42AC-B330-0A0307E7D9E5}" name="ID" dataDxfId="28" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="2" xr3:uid="{482001A2-21E8-4DAF-8F18-394DE1EF23E8}" name="fname" dataDxfId="27" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="3" xr3:uid="{62CAEBE7-2B4E-4A31-A43D-9C1E6783BE94}" name="stage" dataDxfId="26" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="4" xr3:uid="{C3DDC444-FE01-4946-943A-316C89E6C9F5}" name="bdate" dataDxfId="25" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="5" xr3:uid="{0A523B86-F57A-47A9-BC3B-0931AD885DEE}" name="class_name" dataDxfId="24" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="6" xr3:uid="{1684D884-E1CC-43C5-8F89-B64ABE7E4052}" name="school_job" dataDxfId="23" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="7" xr3:uid="{F4FBD935-A0E1-47DA-A8B7-38CE384F94E1}" name="deacon" dataDxfId="22" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="8" xr3:uid="{7AFF96BB-59B7-45A4-A396-B38A52A2FC7D}" name="tel1" dataDxfId="21" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="9" xr3:uid="{166EA85E-C78F-49FB-915D-8286A7D5CA8C}" name="tel2" dataDxfId="20" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="10" xr3:uid="{5807CC3D-4188-4DD0-8D5E-19A1B73F107E}" name="tel3" dataDxfId="19" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="11" xr3:uid="{C06AFBB1-7E3B-4EF5-A160-56495E4FDEBD}" name="tel4" dataDxfId="18" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="12" xr3:uid="{54B8139F-F60D-4904-B893-88E5780B89CF}" name="con_father" dataDxfId="17" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="13" xr3:uid="{8771B84B-CA46-4EDB-AB7D-248236A315FA}" name="address1" dataDxfId="16" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="14" xr3:uid="{ADE2D57B-69BE-4A6C-AAB6-B1FAB40FEB81}" name="address2" dataDxfId="15" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="15" xr3:uid="{A0E272AD-5D56-469A-B900-094133242F8C}" name="address3" dataDxfId="14" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="16" xr3:uid="{C7D87E19-5144-4CDC-B13A-16BD2723305A}" name="address4" dataDxfId="13" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="17" xr3:uid="{A9A56502-942D-4329-8A5B-87A6A6288224}" name="address5" dataDxfId="12" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="18" xr3:uid="{688426DB-69F0-462F-9C69-B38CF0DE0D9C}" name="address6" dataDxfId="11" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="19" xr3:uid="{9C9C5227-3EAC-4FD5-8124-3B0E3870D60F}" name="address7" dataDxfId="10" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="20" xr3:uid="{FC5255B6-2449-45BB-ACC0-0B3B7026D126}" name="God_brothers" dataDxfId="9" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="21" xr3:uid="{0D42DD12-D57B-45DF-A356-DE1BDDEC9C13}" name="notes" dataDxfId="8" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="1" xr3:uid="{56277AF5-8907-42AC-B330-0A0307E7D9E5}" name="ID" dataDxfId="24" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="2" xr3:uid="{482001A2-21E8-4DAF-8F18-394DE1EF23E8}" name="fname" dataDxfId="23" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="3" xr3:uid="{62CAEBE7-2B4E-4A31-A43D-9C1E6783BE94}" name="stage" dataDxfId="22" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="4" xr3:uid="{C3DDC444-FE01-4946-943A-316C89E6C9F5}" name="bdate" dataDxfId="21" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="5" xr3:uid="{0A523B86-F57A-47A9-BC3B-0931AD885DEE}" name="class_name" dataDxfId="20" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="6" xr3:uid="{1684D884-E1CC-43C5-8F89-B64ABE7E4052}" name="school_job" dataDxfId="19" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="7" xr3:uid="{F4FBD935-A0E1-47DA-A8B7-38CE384F94E1}" name="deacon" dataDxfId="18" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="8" xr3:uid="{7AFF96BB-59B7-45A4-A396-B38A52A2FC7D}" name="tel1" dataDxfId="17" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="9" xr3:uid="{166EA85E-C78F-49FB-915D-8286A7D5CA8C}" name="tel2" dataDxfId="16" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="10" xr3:uid="{5807CC3D-4188-4DD0-8D5E-19A1B73F107E}" name="tel3" dataDxfId="15" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="11" xr3:uid="{C06AFBB1-7E3B-4EF5-A160-56495E4FDEBD}" name="tel4" dataDxfId="14" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="12" xr3:uid="{54B8139F-F60D-4904-B893-88E5780B89CF}" name="con_father" dataDxfId="13" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="13" xr3:uid="{8771B84B-CA46-4EDB-AB7D-248236A315FA}" name="address1" dataDxfId="12" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="14" xr3:uid="{ADE2D57B-69BE-4A6C-AAB6-B1FAB40FEB81}" name="address2" dataDxfId="11" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="15" xr3:uid="{A0E272AD-5D56-469A-B900-094133242F8C}" name="address3" dataDxfId="10" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="16" xr3:uid="{C7D87E19-5144-4CDC-B13A-16BD2723305A}" name="address4" dataDxfId="9" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="17" xr3:uid="{A9A56502-942D-4329-8A5B-87A6A6288224}" name="address5" dataDxfId="8" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="18" xr3:uid="{688426DB-69F0-462F-9C69-B38CF0DE0D9C}" name="address6" dataDxfId="7" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="19" xr3:uid="{9C9C5227-3EAC-4FD5-8124-3B0E3870D60F}" name="address7" dataDxfId="6" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="20" xr3:uid="{FC5255B6-2449-45BB-ACC0-0B3B7026D126}" name="God_brothers" dataDxfId="5" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="21" xr3:uid="{0D42DD12-D57B-45DF-A356-DE1BDDEC9C13}" name="notes" dataDxfId="4" dataCellStyle="Normal_Sheet1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5723,24 +5715,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE2741F-E24D-4DF1-B853-B427A7F69F23}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="3" width="12.77734375" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>1341</v>
       </c>
@@ -5760,7 +5752,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1266</v>
       </c>
@@ -5784,7 +5776,7 @@
         <v>القديس بولس الرسول</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5815,7 +5807,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -5845,7 +5837,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1349</v>
       </c>
@@ -5875,7 +5867,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -5905,7 +5897,7 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -5929,7 +5921,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -5953,7 +5945,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -5977,7 +5969,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1256</v>
       </c>
@@ -6001,7 +5993,7 @@
         <v>القديس بولس الرسول</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -6031,7 +6023,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1350</v>
       </c>
@@ -6061,7 +6053,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1351</v>
       </c>
@@ -6092,7 +6084,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1352</v>
       </c>
@@ -6123,7 +6115,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1353</v>
       </c>
@@ -6153,7 +6145,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1354</v>
       </c>
@@ -6183,14 +6175,14 @@
         <v>841</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1355</v>
       </c>
       <c r="B17" t="s">
         <v>1373</v>
       </c>
-      <c r="C17" s="13" t="str" cm="1">
+      <c r="C17" t="str" cm="1">
         <f t="array" ref="C17">IF(_xlfn.XLOOKUP(B17,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B17,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B17,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B17,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B17,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B17,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B17,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B17,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B17,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A17&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الاسم</v>
       </c>
@@ -6202,7 +6194,7 @@
         <f>IF(D17&lt;&gt;"",LOOKUP(D17,Table1[ID],Table1[fname]),"")</f>
         <v xml:space="preserve">ابرام ممدوح كميل </v>
       </c>
-      <c r="F17" s="13" t="str">
+      <c r="F17" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس لوقا الرسول</v>
       </c>
@@ -6213,14 +6205,14 @@
         <v>895</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1356</v>
       </c>
       <c r="B18" t="s">
         <v>1374</v>
       </c>
-      <c r="C18" s="13" t="str" cm="1">
+      <c r="C18" t="str" cm="1">
         <f t="array" ref="C18">IF(_xlfn.XLOOKUP(B18,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B18,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B18,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B18,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B18,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B18,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B18,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B18,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B18,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A18&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الاسم</v>
       </c>
@@ -6232,7 +6224,7 @@
         <f>IF(D18&lt;&gt;"",LOOKUP(D18,Table1[ID],Table1[fname]),"")</f>
         <v xml:space="preserve">بافلي اديب سمير </v>
       </c>
-      <c r="F18" s="13" t="str">
+      <c r="F18" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس بولس الرسول</v>
       </c>
@@ -6243,14 +6235,14 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="13" t="str" cm="1">
+      <c r="C19" t="str" cm="1">
         <f t="array" ref="C19">IF(_xlfn.XLOOKUP(B19,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B19,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B19,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B19,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B19,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B19,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B19,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B19,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B19,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A19&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الاسم</v>
       </c>
@@ -6262,19 +6254,19 @@
         <f>IF(D19&lt;&gt;"",LOOKUP(D19,Table1[ID],Table1[fname]),"")</f>
         <v xml:space="preserve">مارك سامح ابراهيم </v>
       </c>
-      <c r="F19" s="13" t="str">
+      <c r="F19" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس متياس الرسول</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1357</v>
       </c>
       <c r="B20" t="s">
         <v>1317</v>
       </c>
-      <c r="C20" s="13" t="str" cm="1">
+      <c r="C20" t="str" cm="1">
         <f t="array" ref="C20">IF(_xlfn.XLOOKUP(B20,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B20,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B20,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B20,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B20,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B20,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B20,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B20,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B20,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A20&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الموبايل الشخصي</v>
       </c>
@@ -6286,19 +6278,19 @@
         <f>IF(D20&lt;&gt;"",LOOKUP(D20,Table1[ID],Table1[fname]),"")</f>
         <v xml:space="preserve">ميشيل اكرامي حبيب </v>
       </c>
-      <c r="F20" s="13" t="str">
+      <c r="F20" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس بولس الرسول</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1358</v>
       </c>
       <c r="B21" t="s">
         <v>1375</v>
       </c>
-      <c r="C21" s="13" t="str" cm="1">
+      <c r="C21" t="str" cm="1">
         <f t="array" ref="C21">IF(_xlfn.XLOOKUP(B21,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B21,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B21,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B21,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B21,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B21,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B21,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B21,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B21,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A21&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الاسم</v>
       </c>
@@ -6310,19 +6302,19 @@
         <f>IF(D21&lt;&gt;"",LOOKUP(D21,Table1[ID],Table1[fname]),"")</f>
         <v xml:space="preserve">نوفير اسامة حنا </v>
       </c>
-      <c r="F21" s="13" t="str">
+      <c r="F21" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس بولس الرسول</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1359</v>
       </c>
       <c r="B22" t="s">
         <v>1376</v>
       </c>
-      <c r="C22" s="13" t="str" cm="1">
+      <c r="C22" t="str" cm="1">
         <f t="array" ref="C22">IF(_xlfn.XLOOKUP(B22,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B22,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B22,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B22,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B22,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B22,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B22,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B22,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B22,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A22&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الاسم</v>
       </c>
@@ -6334,19 +6326,19 @@
         <f>IF(D22&lt;&gt;"",LOOKUP(D22,Table1[ID],Table1[fname]),"")</f>
         <v xml:space="preserve">يوسف ريمون فؤاد </v>
       </c>
-      <c r="F22" s="13" t="str">
+      <c r="F22" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس بولس الرسول</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="13" t="str" cm="1">
+      <c r="C23" t="str" cm="1">
         <f t="array" ref="C23">IF(_xlfn.XLOOKUP(B23,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B23,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B23,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B23,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B23,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B23,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B23,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B23,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B23,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A23&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الاسم</v>
       </c>
@@ -6358,19 +6350,19 @@
         <f>IF(D23&lt;&gt;"",LOOKUP(D23,Table1[ID],Table1[fname]),"")</f>
         <v>اندرو مخلص بطرس</v>
       </c>
-      <c r="F23" s="13" t="str">
+      <c r="F23" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس مرقس الرسول</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1360</v>
       </c>
       <c r="B24" t="s">
         <v>278</v>
       </c>
-      <c r="C24" s="13" t="str" cm="1">
+      <c r="C24" t="str" cm="1">
         <f t="array" ref="C24">IF(_xlfn.XLOOKUP(B24,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B24,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B24,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B24,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B24,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B24,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B24,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B24,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B24,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A24&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الموبايل الشخصي</v>
       </c>
@@ -6382,19 +6374,19 @@
         <f>IF(D24&lt;&gt;"",LOOKUP(D24,Table1[ID],Table1[fname]),"")</f>
         <v xml:space="preserve">بولا هاني جرجس </v>
       </c>
-      <c r="F24" s="13" t="str">
+      <c r="F24" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس مرقس الرسول</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1361</v>
       </c>
       <c r="B25" t="s">
         <v>1261</v>
       </c>
-      <c r="C25" s="13" t="str" cm="1">
+      <c r="C25" t="str" cm="1">
         <f t="array" ref="C25">IF(_xlfn.XLOOKUP(B25,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B25,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B25,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B25,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B25,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B25,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B25,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B25,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B25,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A25&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الموبايل الشخصي</v>
       </c>
@@ -6406,19 +6398,19 @@
         <f>IF(D25&lt;&gt;"",LOOKUP(D25,Table1[ID],Table1[fname]),"")</f>
         <v>بيشوي مجدي مكرم</v>
       </c>
-      <c r="F25" s="13" t="str">
+      <c r="F25" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس بولس الرسول</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="13" t="str" cm="1">
+      <c r="C26" t="str" cm="1">
         <f t="array" ref="C26">IF(_xlfn.XLOOKUP(B26,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B26,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B26,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B26,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B26,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B26,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B26,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B26,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B26,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A26&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الموبايل الشخصي</v>
       </c>
@@ -6430,19 +6422,19 @@
         <f>IF(D26&lt;&gt;"",LOOKUP(D26,Table1[ID],Table1[fname]),"")</f>
         <v>ماثيو سامح فايز</v>
       </c>
-      <c r="F26" s="13" t="str">
+      <c r="F26" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس مرقس الرسول</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1362</v>
       </c>
       <c r="B27" t="s">
         <v>1300</v>
       </c>
-      <c r="C27" s="13" t="str" cm="1">
+      <c r="C27" t="str" cm="1">
         <f t="array" ref="C27">IF(_xlfn.XLOOKUP(B27,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B27,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B27,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B27,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B27,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B27,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B27,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B27,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B27,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A27&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الموبايل الشخصي</v>
       </c>
@@ -6454,19 +6446,19 @@
         <f>IF(D27&lt;&gt;"",LOOKUP(D27,Table1[ID],Table1[fname]),"")</f>
         <v xml:space="preserve">دانيال شنوده تادرس </v>
       </c>
-      <c r="F27" s="13" t="str">
+      <c r="F27" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس بولس الرسول</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1363</v>
       </c>
       <c r="B28" t="s">
         <v>1377</v>
       </c>
-      <c r="C28" s="13" t="str" cm="1">
+      <c r="C28" t="str" cm="1">
         <f t="array" ref="C28">IF(_xlfn.XLOOKUP(B28,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B28,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B28,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B28,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B28,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B28,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B28,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B28,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B28,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A28&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>مش موجود</v>
       </c>
@@ -6478,19 +6470,19 @@
         <f>IF(D28&lt;&gt;"",LOOKUP(D28,Table1[ID],Table1[fname]),"")</f>
         <v/>
       </c>
-      <c r="F28" s="13" t="str">
+      <c r="F28" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1364</v>
       </c>
       <c r="B29" t="s">
         <v>1378</v>
       </c>
-      <c r="C29" s="13" t="str" cm="1">
+      <c r="C29" t="str" cm="1">
         <f t="array" ref="C29">IF(_xlfn.XLOOKUP(B29,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B29,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B29,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B29,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B29,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B29,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B29,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B29,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B29,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A29&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>مش موجود</v>
       </c>
@@ -6502,19 +6494,19 @@
         <f>IF(D29&lt;&gt;"",LOOKUP(D29,Table1[ID],Table1[fname]),"")</f>
         <v/>
       </c>
-      <c r="F29" s="13" t="str">
+      <c r="F29" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1365</v>
       </c>
       <c r="B30" t="s">
         <v>1379</v>
       </c>
-      <c r="C30" s="13" t="str" cm="1">
+      <c r="C30" t="str" cm="1">
         <f t="array" ref="C30">IF(_xlfn.XLOOKUP(B30,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B30,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B30,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B30,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B30,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B30,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B30,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B30,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B30,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A30&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>مش موجود</v>
       </c>
@@ -6526,16 +6518,16 @@
         <f>IF(D30&lt;&gt;"",LOOKUP(D30,Table1[ID],Table1[fname]),"")</f>
         <v/>
       </c>
-      <c r="F30" s="13" t="str">
+      <c r="F30" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1366</v>
       </c>
-      <c r="C31" s="13" t="str" cm="1">
+      <c r="C31" t="str" cm="1">
         <f t="array" ref="C31">IF(_xlfn.XLOOKUP(B31,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B31,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B31,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B31,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B31,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B31,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B31,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B31,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B31,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A31&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>مش موجود</v>
       </c>
@@ -6547,19 +6539,19 @@
         <f>IF(D31&lt;&gt;"",LOOKUP(D31,Table1[ID],Table1[fname]),"")</f>
         <v/>
       </c>
-      <c r="F31" s="13" t="str">
+      <c r="F31" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1367</v>
       </c>
       <c r="B32" t="s">
         <v>1380</v>
       </c>
-      <c r="C32" s="13" t="str" cm="1">
+      <c r="C32" t="str" cm="1">
         <f t="array" ref="C32">IF(_xlfn.XLOOKUP(B32,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B32,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B32,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B32,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B32,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B32,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B32,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B32,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B32,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A32&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>مش موجود</v>
       </c>
@@ -6571,19 +6563,19 @@
         <f>IF(D32&lt;&gt;"",LOOKUP(D32,Table1[ID],Table1[fname]),"")</f>
         <v/>
       </c>
-      <c r="F32" s="13" t="str">
+      <c r="F32" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1368</v>
       </c>
       <c r="B33" t="s">
         <v>668</v>
       </c>
-      <c r="C33" s="13" t="str" cm="1">
+      <c r="C33" t="str" cm="1">
         <f t="array" ref="C33">IF(_xlfn.XLOOKUP(B33,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B33,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B33,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B33,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B33,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B33,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B33,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B33,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B33,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A33&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الموبايل الشخصي</v>
       </c>
@@ -6595,19 +6587,19 @@
         <f>IF(D33&lt;&gt;"",LOOKUP(D33,Table1[ID],Table1[fname]),"")</f>
         <v>ديفيد صبحي صبحي</v>
       </c>
-      <c r="F33" s="13" t="str">
+      <c r="F33" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس يوحنا الرسول</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1369</v>
       </c>
       <c r="B34" t="s">
         <v>715</v>
       </c>
-      <c r="C34" s="13" t="str" cm="1">
+      <c r="C34" t="str" cm="1">
         <f t="array" ref="C34">IF(_xlfn.XLOOKUP(B34,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B34,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B34,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B34,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B34,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B34,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B34,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B34,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B34,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A34&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الموبايل الشخصي</v>
       </c>
@@ -6619,19 +6611,19 @@
         <f>IF(D34&lt;&gt;"",LOOKUP(D34,Table1[ID],Table1[fname]),"")</f>
         <v>فيلوباتير عماد لطفي ناشد</v>
       </c>
-      <c r="F34" s="13" t="str">
+      <c r="F34" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس يوحنا الرسول</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1370</v>
       </c>
       <c r="B35" t="s">
         <v>726</v>
       </c>
-      <c r="C35" s="13" t="str" cm="1">
+      <c r="C35" t="str" cm="1">
         <f t="array" ref="C35">IF(_xlfn.XLOOKUP(B35,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B35,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B35,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B35,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B35,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B35,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B35,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B35,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B35,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A35&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الموبايل الشخصي</v>
       </c>
@@ -6643,19 +6635,19 @@
         <f>IF(D35&lt;&gt;"",LOOKUP(D35,Table1[ID],Table1[fname]),"")</f>
         <v>كيرلس مراد ماهر</v>
       </c>
-      <c r="F35" s="13" t="str">
+      <c r="F35" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس يوحنا الرسول</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1279</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="13" t="str" cm="1">
+      <c r="C36" t="str" cm="1">
         <f t="array" ref="C36">IF(_xlfn.XLOOKUP(B36,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B36,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B36,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B36,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B36,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B36,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B36,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B36,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B36,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A36&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
         <v>الموبايل الشخصي</v>
       </c>
@@ -6667,25 +6659,265 @@
         <f>IF(D36&lt;&gt;"",LOOKUP(D36,Table1[ID],Table1[fname]),"")</f>
         <v>ابانوب هاني محروس</v>
       </c>
-      <c r="F36" s="13" t="str">
+      <c r="F36" t="str">
         <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
         <v>القديس بولس الرسول</v>
       </c>
     </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C37" s="14" t="str" cm="1">
+        <f t="array" ref="C37">IF(_xlfn.XLOOKUP(B37,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B37,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B37,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B37,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B37,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B37,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B37,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B37,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B37,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A37&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
+        <v>مش موجود</v>
+      </c>
+      <c r="D37" t="str">
+        <f>_xlfn.XLOOKUP(B37,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B37,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B37,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B37,Table1[tel4],Table1[ID],IF(ISNUMBER(_xlfn.XLOOKUP(A37&amp;"*",Table1[fname],Table1[ID],"",2)),_xlfn.XLOOKUP(A37&amp;"*",Table1[fname],Table1[ID],"",2),""),0),0),0),0)</f>
+        <v/>
+      </c>
+      <c r="E37" t="str">
+        <f>IF(D37&lt;&gt;"",LOOKUP(D37,Table1[ID],Table1[fname]),"")</f>
+        <v/>
+      </c>
+      <c r="F37" s="14" t="str">
+        <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C38" s="14" t="str" cm="1">
+        <f t="array" ref="C38">IF(_xlfn.XLOOKUP(B38,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B38,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B38,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B38,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B38,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B38,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B38,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B38,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B38,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A38&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
+        <v>الموبايل الشخصي</v>
+      </c>
+      <c r="D38">
+        <f>_xlfn.XLOOKUP(B38,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B38,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B38,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B38,Table1[tel4],Table1[ID],IF(ISNUMBER(_xlfn.XLOOKUP(A38&amp;"*",Table1[fname],Table1[ID],"",2)),_xlfn.XLOOKUP(A38&amp;"*",Table1[fname],Table1[ID],"",2),""),0),0),0),0)</f>
+        <v>802</v>
+      </c>
+      <c r="E38" t="str">
+        <f>IF(D38&lt;&gt;"",LOOKUP(D38,Table1[ID],Table1[fname]),"")</f>
+        <v>كيرلس ناجي صبحي</v>
+      </c>
+      <c r="F38" s="14" t="str">
+        <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
+        <v>الخدام</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C39" s="14" t="str" cm="1">
+        <f t="array" ref="C39">IF(_xlfn.XLOOKUP(B39,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B39,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B39,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B39,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B39,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B39,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B39,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B39,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B39,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A39&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
+        <v>مش موجود</v>
+      </c>
+      <c r="D39" t="str">
+        <f>_xlfn.XLOOKUP(B39,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B39,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B39,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B39,Table1[tel4],Table1[ID],IF(ISNUMBER(_xlfn.XLOOKUP(A39&amp;"*",Table1[fname],Table1[ID],"",2)),_xlfn.XLOOKUP(A39&amp;"*",Table1[fname],Table1[ID],"",2),""),0),0),0),0)</f>
+        <v/>
+      </c>
+      <c r="E39" t="str">
+        <f>IF(D39&lt;&gt;"",LOOKUP(D39,Table1[ID],Table1[fname]),"")</f>
+        <v/>
+      </c>
+      <c r="F39" s="14" t="str">
+        <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C40" s="14" t="str" cm="1">
+        <f t="array" ref="C40">IF(_xlfn.XLOOKUP(B40,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B40,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B40,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B40,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B40,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B40,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B40,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B40,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B40,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A40&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
+        <v>مش موجود</v>
+      </c>
+      <c r="D40" t="str">
+        <f>_xlfn.XLOOKUP(B40,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B40,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B40,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B40,Table1[tel4],Table1[ID],IF(ISNUMBER(_xlfn.XLOOKUP(A40&amp;"*",Table1[fname],Table1[ID],"",2)),_xlfn.XLOOKUP(A40&amp;"*",Table1[fname],Table1[ID],"",2),""),0),0),0),0)</f>
+        <v/>
+      </c>
+      <c r="E40" t="str">
+        <f>IF(D40&lt;&gt;"",LOOKUP(D40,Table1[ID],Table1[fname]),"")</f>
+        <v/>
+      </c>
+      <c r="F40" s="14" t="str">
+        <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C41" s="14" t="str" cm="1">
+        <f t="array" ref="C41">IF(_xlfn.XLOOKUP(B41,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B41,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B41,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B41,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B41,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B41,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B41,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B41,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B41,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A41&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
+        <v>مش موجود</v>
+      </c>
+      <c r="D41" t="str">
+        <f>_xlfn.XLOOKUP(B41,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B41,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B41,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B41,Table1[tel4],Table1[ID],IF(ISNUMBER(_xlfn.XLOOKUP(A41&amp;"*",Table1[fname],Table1[ID],"",2)),_xlfn.XLOOKUP(A41&amp;"*",Table1[fname],Table1[ID],"",2),""),0),0),0),0)</f>
+        <v/>
+      </c>
+      <c r="E41" t="str">
+        <f>IF(D41&lt;&gt;"",LOOKUP(D41,Table1[ID],Table1[fname]),"")</f>
+        <v/>
+      </c>
+      <c r="F41" s="14" t="str">
+        <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C42" s="14" t="str" cm="1">
+        <f t="array" ref="C42">IF(_xlfn.XLOOKUP(B42,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B42,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B42,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B42,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B42,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B42,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B42,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B42,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B42,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A42&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
+        <v>مش موجود</v>
+      </c>
+      <c r="D42" t="str">
+        <f>_xlfn.XLOOKUP(B42,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B42,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B42,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B42,Table1[tel4],Table1[ID],IF(ISNUMBER(_xlfn.XLOOKUP(A42&amp;"*",Table1[fname],Table1[ID],"",2)),_xlfn.XLOOKUP(A42&amp;"*",Table1[fname],Table1[ID],"",2),""),0),0),0),0)</f>
+        <v/>
+      </c>
+      <c r="E42" t="str">
+        <f>IF(D42&lt;&gt;"",LOOKUP(D42,Table1[ID],Table1[fname]),"")</f>
+        <v/>
+      </c>
+      <c r="F42" s="14" t="str">
+        <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C43" s="14" t="str" cm="1">
+        <f t="array" ref="C43">IF(_xlfn.XLOOKUP(B43,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B43,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B43,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B43,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B43,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B43,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B43,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B43,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B43,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A43&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
+        <v>الموبايل الشخصي</v>
+      </c>
+      <c r="D43">
+        <f>_xlfn.XLOOKUP(B43,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B43,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B43,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B43,Table1[tel4],Table1[ID],IF(ISNUMBER(_xlfn.XLOOKUP(A43&amp;"*",Table1[fname],Table1[ID],"",2)),_xlfn.XLOOKUP(A43&amp;"*",Table1[fname],Table1[ID],"",2),""),0),0),0),0)</f>
+        <v>811</v>
+      </c>
+      <c r="E43" t="str">
+        <f>IF(D43&lt;&gt;"",LOOKUP(D43,Table1[ID],Table1[fname]),"")</f>
+        <v xml:space="preserve">ارساني جرجس نعيم </v>
+      </c>
+      <c r="F43" s="14" t="str">
+        <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
+        <v>القديس بولس الرسول</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>668</v>
+      </c>
+      <c r="C44" s="14" t="str" cm="1">
+        <f t="array" ref="C44">IF(_xlfn.XLOOKUP(B44,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B44,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B44,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B44,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B44,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B44,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B44,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B44,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B44,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A44&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
+        <v>الموبايل الشخصي</v>
+      </c>
+      <c r="D44">
+        <f>_xlfn.XLOOKUP(B44,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B44,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B44,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B44,Table1[tel4],Table1[ID],IF(ISNUMBER(_xlfn.XLOOKUP(A44&amp;"*",Table1[fname],Table1[ID],"",2)),_xlfn.XLOOKUP(A44&amp;"*",Table1[fname],Table1[ID],"",2),""),0),0),0),0)</f>
+        <v>427</v>
+      </c>
+      <c r="E44" t="str">
+        <f>IF(D44&lt;&gt;"",LOOKUP(D44,Table1[ID],Table1[fname]),"")</f>
+        <v>ديفيد صبحي صبحي</v>
+      </c>
+      <c r="F44" s="14" t="str">
+        <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
+        <v>القديس يوحنا الرسول</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C45" s="14" t="str" cm="1">
+        <f t="array" ref="C45">IF(_xlfn.XLOOKUP(B45,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B45,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B45,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B45,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B45,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B45,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B45,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B45,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B45,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A45&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
+        <v>الموبايل الشخصي</v>
+      </c>
+      <c r="D45">
+        <f>_xlfn.XLOOKUP(B45,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B45,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B45,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B45,Table1[tel4],Table1[ID],IF(ISNUMBER(_xlfn.XLOOKUP(A45&amp;"*",Table1[fname],Table1[ID],"",2)),_xlfn.XLOOKUP(A45&amp;"*",Table1[fname],Table1[ID],"",2),""),0),0),0),0)</f>
+        <v>815</v>
+      </c>
+      <c r="E45" t="str">
+        <f>IF(D45&lt;&gt;"",LOOKUP(D45,Table1[ID],Table1[fname]),"")</f>
+        <v xml:space="preserve">بافلي بطرس اليشع </v>
+      </c>
+      <c r="F45" s="14" t="str">
+        <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
+        <v>القديس بولس الرسول</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C46" s="14" t="str" cm="1">
+        <f t="array" ref="C46">IF(_xlfn.XLOOKUP(B46,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B46,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B46,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B46,Table1[tel4],Table1[ID],"",0),0),0),0)&lt;&gt;"",LOOKUP(LOOKUP(Sheet4!B46,_xlfn._xlws.FILTER(Table1[[tel1]:[tel4]],Table1[ID]=_xlfn.XLOOKUP(B46,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B46,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B46,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B46,Table1[tel4],Table1[ID],"",0),0),0),0)),Table1[[#Headers],[tel1]:[tel4]]),_xlfn.ANCHORARRAY(Sheet4!$M$3),Sheet4!$N$3:$N$6),IF(ISNUMBER(_xlfn.XLOOKUP(A46&amp;"*",Table1[fname],Table1[ID],"",2)),"الاسم","مش موجود"))</f>
+        <v>مش موجود</v>
+      </c>
+      <c r="D46" t="str">
+        <f>_xlfn.XLOOKUP(B46,Table1[tel1],Table1[ID],_xlfn.XLOOKUP(B46,Table1[tel2],Table1[ID],_xlfn.XLOOKUP(B46,Table1[tel3],Table1[ID],_xlfn.XLOOKUP(B46,Table1[tel4],Table1[ID],IF(ISNUMBER(_xlfn.XLOOKUP(A46&amp;"*",Table1[fname],Table1[ID],"",2)),_xlfn.XLOOKUP(A46&amp;"*",Table1[fname],Table1[ID],"",2),""),0),0),0),0)</f>
+        <v/>
+      </c>
+      <c r="E46" t="str">
+        <f>IF(D46&lt;&gt;"",LOOKUP(D46,Table1[ID],Table1[fname]),"")</f>
+        <v/>
+      </c>
+      <c r="F46" s="14" t="str">
+        <f>IF(Table2[[#This Row],[اللي لقيته]]&lt;&gt;"مش موجود",_xlfn.IFNA(IF((Table2[[#This Row],[ID]]-FLOOR(Table2[[#This Row],[ID]],100))&lt;6,"الخدام",LOOKUP(FLOOR(Table2[[#This Row],[ID]],100),$M$11:$M$18,$N$11:$N$18)),"الخدام"),"")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A36">
-    <cfRule type="expression" dxfId="7" priority="2">
+  <conditionalFormatting sqref="A1:A46">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>C1="الاسم"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B36">
-    <cfRule type="expression" dxfId="6" priority="1">
+  <conditionalFormatting sqref="B1:B46">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>_xlfn.XLOOKUP(C1,$N$3:$N$6,$M$3:$M$6,"nn")&lt;&gt;"nn"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:F36">
-    <cfRule type="expression" dxfId="5" priority="3">
+  <conditionalFormatting sqref="C1:F46">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$C1="مش موجود"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6704,18 +6936,17 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" customWidth="1"/>
-    <col min="13" max="19" width="10.109375" customWidth="1"/>
-    <col min="20" max="20" width="14.109375" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="19" width="10.140625" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
@@ -6780,7 +7011,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -6845,7 +7076,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -6910,7 +7141,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -6975,7 +7206,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -7040,7 +7271,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -7105,7 +7336,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -7170,7 +7401,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>102</v>
       </c>
@@ -7235,7 +7466,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>103</v>
       </c>
@@ -7300,7 +7531,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>104</v>
       </c>
@@ -7365,7 +7596,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>113</v>
       </c>
@@ -7430,7 +7661,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>114</v>
       </c>
@@ -7495,7 +7726,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>115</v>
       </c>
@@ -7560,7 +7791,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>116</v>
       </c>
@@ -7625,7 +7856,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>118</v>
       </c>
@@ -7690,7 +7921,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>119</v>
       </c>
@@ -7755,7 +7986,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>120</v>
       </c>
@@ -7820,7 +8051,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>121</v>
       </c>
@@ -7885,7 +8116,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>122</v>
       </c>
@@ -7950,7 +8181,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>123</v>
       </c>
@@ -8015,7 +8246,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>124</v>
       </c>
@@ -8080,7 +8311,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>125</v>
       </c>
@@ -8145,7 +8376,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>126</v>
       </c>
@@ -8210,7 +8441,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>127</v>
       </c>
@@ -8275,7 +8506,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>128</v>
       </c>
@@ -8340,7 +8571,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>129</v>
       </c>
@@ -8405,7 +8636,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>130</v>
       </c>
@@ -8470,7 +8701,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>131</v>
       </c>
@@ -8535,7 +8766,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>132</v>
       </c>
@@ -8600,7 +8831,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>133</v>
       </c>
@@ -8665,7 +8896,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>134</v>
       </c>
@@ -8730,7 +8961,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>135</v>
       </c>
@@ -8795,7 +9026,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>136</v>
       </c>
@@ -8860,7 +9091,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>137</v>
       </c>
@@ -8925,7 +9156,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>138</v>
       </c>
@@ -8990,7 +9221,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>139</v>
       </c>
@@ -9055,7 +9286,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>140</v>
       </c>
@@ -9120,7 +9351,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>202</v>
       </c>
@@ -9185,7 +9416,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>203</v>
       </c>
@@ -9250,7 +9481,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>204</v>
       </c>
@@ -9315,7 +9546,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>210</v>
       </c>
@@ -9380,7 +9611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>211</v>
       </c>
@@ -9445,7 +9676,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>212</v>
       </c>
@@ -9510,7 +9741,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>214</v>
       </c>
@@ -9575,7 +9806,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>215</v>
       </c>
@@ -9640,7 +9871,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>216</v>
       </c>
@@ -9705,7 +9936,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>217</v>
       </c>
@@ -9770,7 +10001,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>218</v>
       </c>
@@ -9835,7 +10066,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>219</v>
       </c>
@@ -9900,7 +10131,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>220</v>
       </c>
@@ -9965,7 +10196,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>221</v>
       </c>
@@ -10030,7 +10261,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>222</v>
       </c>
@@ -10095,7 +10326,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>223</v>
       </c>
@@ -10160,7 +10391,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>224</v>
       </c>
@@ -10225,7 +10456,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>225</v>
       </c>
@@ -10290,7 +10521,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>226</v>
       </c>
@@ -10355,7 +10586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>227</v>
       </c>
@@ -10420,7 +10651,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>228</v>
       </c>
@@ -10485,7 +10716,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>229</v>
       </c>
@@ -10550,7 +10781,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>230</v>
       </c>
@@ -10615,7 +10846,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>231</v>
       </c>
@@ -10680,7 +10911,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>232</v>
       </c>
@@ -10745,7 +10976,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>234</v>
       </c>
@@ -10810,7 +11041,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>235</v>
       </c>
@@ -10875,7 +11106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>236</v>
       </c>
@@ -10940,7 +11171,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>237</v>
       </c>
@@ -11005,7 +11236,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>239</v>
       </c>
@@ -11070,7 +11301,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>240</v>
       </c>
@@ -11135,7 +11366,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>241</v>
       </c>
@@ -11200,7 +11431,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>242</v>
       </c>
@@ -11265,7 +11496,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>243</v>
       </c>
@@ -11330,7 +11561,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>244</v>
       </c>
@@ -11395,7 +11626,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>245</v>
       </c>
@@ -11460,7 +11691,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>246</v>
       </c>
@@ -11525,7 +11756,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>247</v>
       </c>
@@ -11590,7 +11821,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>248</v>
       </c>
@@ -11655,7 +11886,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>249</v>
       </c>
@@ -11720,7 +11951,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>250</v>
       </c>
@@ -11785,7 +12016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>251</v>
       </c>
@@ -11850,7 +12081,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>252</v>
       </c>
@@ -11915,7 +12146,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>303</v>
       </c>
@@ -11980,7 +12211,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>304</v>
       </c>
@@ -12045,7 +12276,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>310</v>
       </c>
@@ -12110,7 +12341,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>311</v>
       </c>
@@ -12175,7 +12406,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>312</v>
       </c>
@@ -12240,7 +12471,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>313</v>
       </c>
@@ -12305,7 +12536,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>314</v>
       </c>
@@ -12370,7 +12601,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>315</v>
       </c>
@@ -12435,7 +12666,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>317</v>
       </c>
@@ -12500,7 +12731,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>318</v>
       </c>
@@ -12565,7 +12796,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>319</v>
       </c>
@@ -12630,7 +12861,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>321</v>
       </c>
@@ -12695,7 +12926,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>322</v>
       </c>
@@ -12760,7 +12991,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>323</v>
       </c>
@@ -12825,7 +13056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>324</v>
       </c>
@@ -12890,7 +13121,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>325</v>
       </c>
@@ -12955,7 +13186,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>327</v>
       </c>
@@ -13020,7 +13251,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>328</v>
       </c>
@@ -13085,7 +13316,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="99" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>329</v>
       </c>
@@ -13150,7 +13381,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="100" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>330</v>
       </c>
@@ -13215,7 +13446,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>333</v>
       </c>
@@ -13280,7 +13511,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>334</v>
       </c>
@@ -13345,7 +13576,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>336</v>
       </c>
@@ -13410,7 +13641,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>337</v>
       </c>
@@ -13475,7 +13706,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>338</v>
       </c>
@@ -13540,7 +13771,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="106" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>339</v>
       </c>
@@ -13605,7 +13836,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>340</v>
       </c>
@@ -13670,7 +13901,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="108" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>341</v>
       </c>
@@ -13735,7 +13966,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>342</v>
       </c>
@@ -13800,7 +14031,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="110" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>343</v>
       </c>
@@ -13865,7 +14096,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>344</v>
       </c>
@@ -13930,7 +14161,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="112" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>345</v>
       </c>
@@ -13995,7 +14226,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="113" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>346</v>
       </c>
@@ -14060,7 +14291,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>347</v>
       </c>
@@ -14125,7 +14356,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>348</v>
       </c>
@@ -14190,7 +14421,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>349</v>
       </c>
@@ -14255,7 +14486,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="117" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>401</v>
       </c>
@@ -14320,7 +14551,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="118" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>402</v>
       </c>
@@ -14385,7 +14616,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>403</v>
       </c>
@@ -14450,7 +14681,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>404</v>
       </c>
@@ -14515,7 +14746,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="121" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>410</v>
       </c>
@@ -14580,7 +14811,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="122" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>411</v>
       </c>
@@ -14645,7 +14876,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="123" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>412</v>
       </c>
@@ -14710,7 +14941,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="124" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>413</v>
       </c>
@@ -14775,7 +15006,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="125" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>415</v>
       </c>
@@ -14840,7 +15071,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="126" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>416</v>
       </c>
@@ -14905,7 +15136,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="127" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>417</v>
       </c>
@@ -14970,7 +15201,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>419</v>
       </c>
@@ -15035,7 +15266,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="129" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>420</v>
       </c>
@@ -15100,7 +15331,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="130" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>421</v>
       </c>
@@ -15165,7 +15396,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="131" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>422</v>
       </c>
@@ -15230,7 +15461,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="132" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>423</v>
       </c>
@@ -15295,7 +15526,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="133" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>424</v>
       </c>
@@ -15360,7 +15591,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="134" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>426</v>
       </c>
@@ -15425,7 +15656,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="135" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>427</v>
       </c>
@@ -15490,7 +15721,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="136" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>428</v>
       </c>
@@ -15555,7 +15786,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="137" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>429</v>
       </c>
@@ -15620,7 +15851,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="138" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>430</v>
       </c>
@@ -15685,7 +15916,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="139" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>431</v>
       </c>
@@ -15750,7 +15981,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="140" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>432</v>
       </c>
@@ -15815,7 +16046,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="141" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>433</v>
       </c>
@@ -15880,7 +16111,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="142" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>434</v>
       </c>
@@ -15945,7 +16176,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="143" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>435</v>
       </c>
@@ -16010,7 +16241,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="144" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>436</v>
       </c>
@@ -16075,7 +16306,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>437</v>
       </c>
@@ -16140,7 +16371,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>438</v>
       </c>
@@ -16205,7 +16436,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>439</v>
       </c>
@@ -16270,7 +16501,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>440</v>
       </c>
@@ -16335,7 +16566,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="149" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>441</v>
       </c>
@@ -16400,7 +16631,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="150" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>442</v>
       </c>
@@ -16465,7 +16696,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="151" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>443</v>
       </c>
@@ -16530,7 +16761,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="152" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>444</v>
       </c>
@@ -16595,7 +16826,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="153" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>445</v>
       </c>
@@ -16660,7 +16891,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>446</v>
       </c>
@@ -16725,7 +16956,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>448</v>
       </c>
@@ -16790,7 +17021,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="156" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>449</v>
       </c>
@@ -16855,7 +17086,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="157" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>450</v>
       </c>
@@ -16920,7 +17151,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="158" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>451</v>
       </c>
@@ -16985,7 +17216,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="159" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>502</v>
       </c>
@@ -17050,7 +17281,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>503</v>
       </c>
@@ -17115,7 +17346,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="161" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>504</v>
       </c>
@@ -17180,7 +17411,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="162" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>510</v>
       </c>
@@ -17245,7 +17476,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="163" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>512</v>
       </c>
@@ -17310,7 +17541,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="164" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>513</v>
       </c>
@@ -17375,7 +17606,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="165" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>514</v>
       </c>
@@ -17440,7 +17671,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="166" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>515</v>
       </c>
@@ -17505,7 +17736,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="167" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>516</v>
       </c>
@@ -17570,7 +17801,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="168" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>519</v>
       </c>
@@ -17635,7 +17866,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="169" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>520</v>
       </c>
@@ -17700,7 +17931,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="170" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>521</v>
       </c>
@@ -17765,7 +17996,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="171" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>523</v>
       </c>
@@ -17830,7 +18061,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="172" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>524</v>
       </c>
@@ -17895,7 +18126,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="173" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>525</v>
       </c>
@@ -17960,7 +18191,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="174" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>526</v>
       </c>
@@ -18025,7 +18256,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="175" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>528</v>
       </c>
@@ -18090,7 +18321,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="176" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>529</v>
       </c>
@@ -18155,7 +18386,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="177" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>532</v>
       </c>
@@ -18220,7 +18451,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="178" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>602</v>
       </c>
@@ -18285,7 +18516,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="179" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>603</v>
       </c>
@@ -18350,7 +18581,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="180" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>610</v>
       </c>
@@ -18415,7 +18646,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="181" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>611</v>
       </c>
@@ -18480,7 +18711,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="182" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>612</v>
       </c>
@@ -18545,7 +18776,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="183" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>613</v>
       </c>
@@ -18610,7 +18841,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="184" spans="1:21" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>614</v>
       </c>
@@ -18675,7 +18906,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="185" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>615</v>
       </c>
@@ -18740,7 +18971,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="186" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>616</v>
       </c>
@@ -18805,7 +19036,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="187" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>617</v>
       </c>
@@ -18870,7 +19101,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="188" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>618</v>
       </c>
@@ -18935,7 +19166,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="189" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>619</v>
       </c>
@@ -19000,7 +19231,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="190" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>620</v>
       </c>
@@ -19065,7 +19296,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="191" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>621</v>
       </c>
@@ -19130,7 +19361,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="192" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>702</v>
       </c>
@@ -19195,7 +19426,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="193" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>703</v>
       </c>
@@ -19260,7 +19491,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="194" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>710</v>
       </c>
@@ -19325,7 +19556,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="195" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>711</v>
       </c>
@@ -19390,7 +19621,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="196" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>712</v>
       </c>
@@ -19455,7 +19686,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="197" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>713</v>
       </c>
@@ -19520,7 +19751,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="198" spans="1:21" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:21" ht="270" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>714</v>
       </c>
@@ -19585,7 +19816,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="199" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>715</v>
       </c>
@@ -19650,7 +19881,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="200" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>716</v>
       </c>
@@ -19715,7 +19946,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="201" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>717</v>
       </c>
@@ -19780,7 +20011,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="202" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>718</v>
       </c>
@@ -19845,7 +20076,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="203" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>719</v>
       </c>
@@ -19910,7 +20141,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="204" spans="1:21" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>720</v>
       </c>
@@ -19975,7 +20206,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="205" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>721</v>
       </c>
@@ -20040,7 +20271,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="206" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>722</v>
       </c>
@@ -20105,7 +20336,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="207" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>723</v>
       </c>
@@ -20170,7 +20401,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="208" spans="1:21" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:21" ht="345" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>724</v>
       </c>
@@ -20235,7 +20466,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="209" spans="1:21" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:21" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>725</v>
       </c>
@@ -20300,7 +20531,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="210" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>726</v>
       </c>
@@ -20365,7 +20596,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="211" spans="1:21" ht="144" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:21" ht="165" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>727</v>
       </c>
@@ -20430,7 +20661,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:21" ht="195" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>728</v>
       </c>
@@ -20495,7 +20726,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="213" spans="1:21" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>729</v>
       </c>
@@ -20560,7 +20791,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="214" spans="1:21" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>730</v>
       </c>
@@ -20625,7 +20856,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="215" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>731</v>
       </c>
@@ -20690,7 +20921,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="216" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>732</v>
       </c>
@@ -20755,7 +20986,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="217" spans="1:21" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:21" ht="180" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>734</v>
       </c>
@@ -20820,7 +21051,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="218" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>735</v>
       </c>
@@ -20885,7 +21116,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="219" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>736</v>
       </c>
@@ -20950,7 +21181,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="220" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:21" ht="120" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>737</v>
       </c>
@@ -21015,7 +21246,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="221" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>738</v>
       </c>
@@ -21080,7 +21311,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="222" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>739</v>
       </c>
@@ -21145,7 +21376,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="223" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>740</v>
       </c>
@@ -21210,7 +21441,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="224" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>741</v>
       </c>
@@ -21275,7 +21506,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="225" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>742</v>
       </c>
@@ -21340,7 +21571,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="226" spans="1:21" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:21" ht="165" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>743</v>
       </c>
@@ -21405,7 +21636,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="227" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>744</v>
       </c>
@@ -21470,7 +21701,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="228" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>745</v>
       </c>
@@ -21535,7 +21766,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="229" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>746</v>
       </c>
@@ -21600,7 +21831,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="230" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>802</v>
       </c>
@@ -21665,7 +21896,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="231" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>803</v>
       </c>
@@ -21730,7 +21961,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="232" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>810</v>
       </c>
@@ -21795,7 +22026,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="233" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
         <v>811</v>
       </c>
@@ -21860,7 +22091,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="234" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>813</v>
       </c>
@@ -21925,7 +22156,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="235" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <v>814</v>
       </c>
@@ -21990,7 +22221,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="236" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <v>815</v>
       </c>
@@ -22055,7 +22286,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="237" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>816</v>
       </c>
@@ -22120,7 +22351,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="238" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <v>817</v>
       </c>
@@ -22185,7 +22416,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="239" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>818</v>
       </c>
@@ -22250,7 +22481,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="240" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <v>819</v>
       </c>
@@ -22315,7 +22546,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="241" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <v>820</v>
       </c>
@@ -22380,7 +22611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <v>821</v>
       </c>
@@ -22445,7 +22676,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="243" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <v>822</v>
       </c>
@@ -22510,7 +22741,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="244" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <v>823</v>
       </c>
@@ -22575,7 +22806,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="245" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <v>824</v>
       </c>
@@ -22640,7 +22871,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="246" spans="1:21" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:21" ht="195" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <v>825</v>
       </c>
@@ -22705,7 +22936,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="247" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <v>826</v>
       </c>
@@ -22770,7 +23001,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="248" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
         <v>827</v>
       </c>
@@ -22835,7 +23066,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
         <v>828</v>
       </c>
@@ -22900,7 +23131,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="250" spans="1:21" ht="144" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:21" ht="150" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <v>829</v>
       </c>
@@ -22965,7 +23196,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="251" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <v>830</v>
       </c>
@@ -23030,7 +23261,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="252" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
         <v>831</v>
       </c>
@@ -23095,7 +23326,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="253" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <v>832</v>
       </c>
@@ -23160,7 +23391,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="254" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <v>833</v>
       </c>
@@ -23225,7 +23456,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="255" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <v>834</v>
       </c>
@@ -23290,7 +23521,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="256" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <v>835</v>
       </c>
@@ -23355,7 +23586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="257" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <v>836</v>
       </c>
@@ -23420,7 +23651,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="258" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
         <v>837</v>
       </c>
@@ -23485,7 +23716,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="259" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
         <v>838</v>
       </c>
@@ -23550,7 +23781,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="260" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
         <v>839</v>
       </c>
@@ -23615,7 +23846,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="261" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
         <v>840</v>
       </c>
@@ -23680,7 +23911,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="262" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
         <v>841</v>
       </c>
@@ -23745,7 +23976,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="263" spans="1:21" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
         <v>842</v>
       </c>
@@ -23810,7 +24041,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="264" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
         <v>843</v>
       </c>
@@ -23875,7 +24106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="265" spans="1:21" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
         <v>844</v>
       </c>
@@ -23940,7 +24171,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="266" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
         <v>845</v>
       </c>
@@ -24005,7 +24236,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="267" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
         <v>846</v>
       </c>
@@ -24070,7 +24301,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="268" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
         <v>847</v>
       </c>
@@ -24135,7 +24366,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="269" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
         <v>848</v>
       </c>
@@ -24200,7 +24431,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="270" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A270" s="2">
         <v>849</v>
       </c>
@@ -24265,7 +24496,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="271" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A271" s="2">
         <v>850</v>
       </c>
@@ -24330,7 +24561,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="272" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="2">
         <v>851</v>
       </c>
@@ -24395,7 +24626,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="273" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A273" s="2">
         <v>852</v>
       </c>
@@ -24460,7 +24691,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="274" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A274" s="2">
         <v>853</v>
       </c>
@@ -24525,7 +24756,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="275" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" s="2">
         <v>854</v>
       </c>
@@ -24590,7 +24821,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="276" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A276" s="2">
         <v>855</v>
       </c>
@@ -24655,7 +24886,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="277" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A277" s="2">
         <v>856</v>
       </c>
@@ -24720,7 +24951,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="278" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A278" s="2">
         <v>857</v>
       </c>
@@ -24785,7 +25016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="279" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A279" s="2">
         <v>858</v>
       </c>
@@ -24850,7 +25081,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="280" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A280" s="2">
         <v>859</v>
       </c>
@@ -24915,7 +25146,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="281" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A281" s="2">
         <v>860</v>
       </c>
@@ -24980,7 +25211,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="282" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A282" s="2">
         <v>861</v>
       </c>
@@ -25045,7 +25276,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="283" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A283" s="2">
         <v>862</v>
       </c>
@@ -25110,7 +25341,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="284" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A284" s="2">
         <v>863</v>
       </c>
@@ -25175,7 +25406,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="285" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A285" s="2">
         <v>864</v>
       </c>
@@ -25240,7 +25471,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="286" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A286" s="2">
         <v>865</v>
       </c>
@@ -25305,7 +25536,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="287" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A287" s="2">
         <v>866</v>
       </c>
@@ -25370,7 +25601,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="288" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
         <v>867</v>
       </c>
@@ -25435,7 +25666,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="289" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A289" s="2">
         <v>868</v>
       </c>
@@ -25500,7 +25731,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="290" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A290" s="2">
         <v>869</v>
       </c>
@@ -25565,7 +25796,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="291" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A291" s="2">
         <v>870</v>
       </c>
@@ -25630,7 +25861,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A292" s="2">
         <v>871</v>
       </c>
@@ -25695,7 +25926,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="293" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A293" s="2">
         <v>872</v>
       </c>
@@ -25760,7 +25991,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="294" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A294" s="2">
         <v>873</v>
       </c>
@@ -25825,7 +26056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="295" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A295" s="2">
         <v>874</v>
       </c>
@@ -25890,7 +26121,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="296" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A296" s="2">
         <v>875</v>
       </c>
@@ -25955,7 +26186,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="297" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
         <v>876</v>
       </c>
@@ -26020,7 +26251,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="298" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A298" s="2">
         <v>877</v>
       </c>
@@ -26085,7 +26316,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="299" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A299" s="2">
         <v>878</v>
       </c>
@@ -26150,7 +26381,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="300" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A300" s="2">
         <v>879</v>
       </c>
@@ -26215,7 +26446,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="301" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A301" s="2">
         <v>880</v>
       </c>
@@ -26280,7 +26511,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="302" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A302" s="2">
         <v>881</v>
       </c>
@@ -26345,7 +26576,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="303" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A303" s="2">
         <v>882</v>
       </c>
@@ -26410,7 +26641,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="304" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A304" s="2">
         <v>883</v>
       </c>
@@ -26475,7 +26706,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="305" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A305" s="6">
         <v>900</v>
       </c>

</xml_diff>